<commit_message>
Remove news article type, remove CRC database
</commit_message>
<xml_diff>
--- a/LibGuides Resource Batch Update Template.xlsx
+++ b/LibGuides Resource Batch Update Template.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="5RE6xrFWHpdlAkJfS9HADn/SIC+JtRKaYbn6PTgMCsE="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="kDucXslZAO5/gpoo5Oa8FJ/2WGUNnPBglUUIPPLi67M="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="212">
   <si>
     <t>FILLING OUT TEMPLATE INSTRUCTIONS</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>LIBRARIAN REVIEW</t>
+  </si>
+  <si>
+    <t>INTERNAL NOTE</t>
   </si>
   <si>
     <t>ACCESS MODES</t>
@@ -311,6 +314,10 @@
 e.g. Adding a review to this…</t>
   </si>
   <si>
+    <t>Field Type: Text Area
+Field Info: Char. Limit is 1000</t>
+  </si>
+  <si>
     <t>Field Type: Multi Select
 Field Info: Access Mode must exist in the system. Values delimited with semi-colon.
 e.g. Public; No Restricted</t>
@@ -357,7 +364,7 @@
     <t>Top-rated for international news.</t>
   </si>
   <si>
-    <t>Full text;News articles;Non-Fiction;Digital</t>
+    <t>Non-Fiction;Digital</t>
   </si>
   <si>
     <t>News</t>
@@ -429,7 +436,7 @@
     <t>Follett</t>
   </si>
   <si>
-    <t>Full text;Fiction;Non-Fiction;Physical</t>
+    <t>Fiction;Non-Fiction;Physical</t>
   </si>
   <si>
     <t>English;Multi-Subject</t>
@@ -456,7 +463,7 @@
     <t>Sora</t>
   </si>
   <si>
-    <t>Full text;Fiction;Digital</t>
+    <t>Fiction;Digital</t>
   </si>
   <si>
     <t>English</t>
@@ -477,9 +484,6 @@
     <t>Gale</t>
   </si>
   <si>
-    <t>Full text;Non-Fiction;Digital</t>
-  </si>
-  <si>
     <t>Multi-Subject</t>
   </si>
   <si>
@@ -522,19 +526,9 @@
     <t>jstor</t>
   </si>
   <si>
-    <t>Canadian Reference Centre</t>
-  </si>
-  <si>
-    <t>Hide</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/document/d/1sbm51hiZk9YNsdgIUZjv-foj_ZW0PTgNQ_gTS2seW1s/edit?tab=t.0</t>
-  </si>
-  <si>
-    <t>canadian-reference-centre</t>
-  </si>
-  <si>
-    <t>EBSCO</t>
+    <t>Academic journals and eBooks:&lt;br /&gt;
+ · 28,000 peer-reviewed academic journals, all full-text.&lt;br /&gt;
+ · 84,500 scholarly ebooks from university publishers.</t>
   </si>
   <si>
     <t>Bloom’s Literary Reference Online</t>
@@ -711,7 +705,7 @@
     <t>https://docs.google.com/presentation/d/1PvBszQUbrUD_TIihGIdszuRqYyJNZGZxL5mzQerCCoc/preview?rm=minimal#slide=id.g3373fedb5a9_0_9</t>
   </si>
   <si>
-    <t>Resources/flipster</t>
+    <t>resources/flipster</t>
   </si>
   <si>
     <t>flipster</t>
@@ -724,7 +718,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -750,13 +744,9 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="4">
@@ -891,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -933,18 +923,28 @@
     </xf>
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2589,977 +2589,1225 @@
       <c r="Y1" s="19" t="s">
         <v>60</v>
       </c>
+      <c r="Z1" s="20" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="2" ht="96.75" customHeight="1">
-      <c r="A2" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="I2" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="J2" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="K2" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="L2" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="N2" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="O2" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="P2" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="Q2" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="R2" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="T2" s="21" t="s">
+      <c r="S2" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="T2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="U2" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="V2" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="X2" s="21" t="s">
+      <c r="W2" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="Y2" s="21" t="s">
+      <c r="X2" s="22" t="s">
         <v>85</v>
+      </c>
+      <c r="Y2" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="22">
+      <c r="A3" s="24">
         <v>3.7423315E7</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="C3" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="D3" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="E3" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="F3" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="G3" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="L3" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="M3" s="22" t="s">
+      <c r="H3" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="L3" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="N3" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="S3" s="22" t="s">
+      <c r="O3" s="25"/>
+      <c r="P3" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="W3" s="22" t="s">
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25" t="s">
         <v>99</v>
       </c>
+      <c r="S3" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="22">
+      <c r="A4" s="24">
         <v>3.7423316E7</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="B4" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="N4" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="P4" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="R4" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="W4" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="22">
+      <c r="A5" s="24">
         <v>3.7423329E7</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="22" t="s">
+      <c r="B5" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="E5" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="L5" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="P5" s="22" t="s">
+      <c r="M5" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="R5" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="W5" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="N5" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="22">
+      <c r="A6" s="24">
         <v>3.742343E7</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="F6" s="22" t="s">
+      <c r="B6" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="H6" s="22" t="s">
+      <c r="E6" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="F6" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="H6" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="L6" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="T6" s="22" t="s">
+      <c r="M6" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="W6" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="N6" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="22">
+      <c r="A7" s="24">
         <v>3.7423431E7</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="F7" s="22" t="s">
+      <c r="B7" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H7" s="22" t="s">
+      <c r="E7" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="F7" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="H7" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="L7" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="W7" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="M7" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="22">
+      <c r="A8" s="24">
         <v>3.7423432E7</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="22" t="s">
+      <c r="B8" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="H8" s="22" t="s">
+      <c r="E8" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="F8" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="H8" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="W8" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="M8" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N8" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="22">
+      <c r="A9" s="24">
         <v>3.7423433E7</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="22" t="s">
+      <c r="B9" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="C9" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="E9" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="F9" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="L9" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="M9" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" s="22" t="s">
+      <c r="H9" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="W9" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="M9" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="22">
+      <c r="A10" s="24">
         <v>3.7423434E7</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="22" t="s">
+      <c r="B10" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="C10" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="E10" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="F10" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="L10" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="M10" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N10" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="W10" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H10" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N10" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="22">
+      <c r="A11" s="24">
         <v>3.7423435E7</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="22" t="s">
+      <c r="B11" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="C11" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="E11" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="F11" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="L11" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="M11" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N11" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="W11" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H11" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="L11" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="22">
-        <v>3.7423436E7</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="22" t="s">
+      <c r="A12" s="24">
+        <v>3.7423437E7</v>
+      </c>
+      <c r="B12" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="C12" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="E12" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="F12" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="M12" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N12" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="W12" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H12" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M12" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="22">
-        <v>3.7423437E7</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="F13" s="22" t="s">
+      <c r="A13" s="24">
+        <v>3.7423438E7</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="H13" s="22" t="s">
+      <c r="E13" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="L13" s="22" t="s">
+      <c r="F13" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="M13" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N13" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="W13" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H13" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="M13" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="22">
-        <v>3.7423438E7</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="F14" s="22" t="s">
+      <c r="A14" s="24">
+        <v>3.7423439E7</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="K14" s="22" t="s">
+      <c r="E14" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="L14" s="22" t="s">
+      <c r="F14" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="M14" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N14" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="W14" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H14" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="M14" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="25"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="22">
-        <v>3.7423439E7</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" s="22" t="s">
+      <c r="A15" s="24">
+        <v>3.742344E7</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="E15" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="L15" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="H15" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="L15" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="M15" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N15" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="W15" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="M15" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N15" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y15" s="25"/>
+      <c r="Z15" s="25"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="22">
-        <v>3.742344E7</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="F16" s="22" t="s">
+      <c r="A16" s="24">
+        <v>3.7423441E7</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="H16" s="22" t="s">
+      <c r="E16" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="F16" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="L16" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="M16" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N16" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="W16" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H16" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="22">
-        <v>3.7423441E7</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="22" t="s">
+      <c r="A17" s="24">
+        <v>3.7423442E7</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="C17" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="E17" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="F17" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="L17" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N17" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="W17" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H17" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="M17" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="22">
-        <v>3.7423442E7</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="22" t="s">
+      <c r="A18" s="24">
+        <v>3.7423443E7</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="M18" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N18" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="F18" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="L18" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="M18" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N18" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="W18" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="25"/>
+      <c r="X18" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y18" s="25"/>
+      <c r="Z18" s="25"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="22">
-        <v>3.7423443E7</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="22" t="s">
+      <c r="A19" s="24">
+        <v>3.7423444E7</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="C19" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="E19" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="F19" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="L19" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="M19" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N19" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="W19" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H19" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="M19" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
+      <c r="V19" s="25"/>
+      <c r="W19" s="25"/>
+      <c r="X19" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y19" s="25"/>
+      <c r="Z19" s="25"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="22">
-        <v>3.7423444E7</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="22" t="s">
+      <c r="A20" s="24">
+        <v>3.7423445E7</v>
+      </c>
+      <c r="B20" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="C20" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="E20" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="F20" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="L20" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="M20" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N20" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="W20" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H20" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="M20" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N20" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="22">
-        <v>3.7423445E7</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="22" t="s">
+      <c r="A21" s="24">
+        <v>3.7423446E7</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="C21" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="E21" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="F21" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="L21" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="M21" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N21" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="W21" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H21" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="L21" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="M21" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N21" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="U21" s="25"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y21" s="25"/>
+      <c r="Z21" s="25"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="22">
-        <v>3.7423446E7</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="F22" s="22" t="s">
+      <c r="A22" s="24">
+        <v>3.7458513E7</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G22" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="L22" s="22" t="s">
+      <c r="E22" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="M22" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N22" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="T22" s="22" t="s">
+      <c r="F22" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="W22" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="H22" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="L22" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="M22" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N22" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="25"/>
+      <c r="V22" s="25"/>
+      <c r="W22" s="25"/>
+      <c r="X22" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y22" s="25"/>
+      <c r="Z22" s="25"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="22">
-        <v>3.7458513E7</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="F23" s="22" t="s">
+      <c r="A23" s="24">
+        <v>3.7463802E7</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="H23" s="22" t="s">
+      <c r="E23" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="L23" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="K23" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="L23" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="M23" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="N23" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="P23" s="22" t="s">
+      <c r="M23" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="W23" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="N23" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="22">
-        <v>3.7463802E7</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="H24" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="L24" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="N24" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="W24" s="22" t="s">
-        <v>99</v>
-      </c>
-    </row>
+    <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
     <row r="26" ht="14.25" customHeight="1"/>
     <row r="27" ht="14.25" customHeight="1"/>
@@ -4535,14 +4783,10 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="R5"/>
-  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Follett Customization, Bootstrap 4 > 5 guide fix, database update,  header link update
</commit_message>
<xml_diff>
--- a/LibGuides Resource Batch Update Template.xlsx
+++ b/LibGuides Resource Batch Update Template.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="211">
   <si>
     <t>FILLING OUT TEMPLATE INSTRUCTIONS</t>
   </si>
@@ -418,7 +418,7 @@
     <t>https://d1qywhc7l90rsa.cloudfront.net/customers/10289/images/Screenshot_2024-09-10_at_11.20.02%E2%80%AFAM.png</t>
   </si>
   <si>
-    <t>Follett Destiny</t>
+    <t>Book Catalogue</t>
   </si>
   <si>
     <t>https://yorkhouse.follettdestiny.ca/</t>
@@ -672,13 +672,10 @@
     <t>national-film-board-nfb</t>
   </si>
   <si>
-    <t>Log in with your school google account. NFB films can be played on campus without logging in (because we're using IP address authentication). We have an NFB Education licence and, therefore, can make use of the resources available on nfb.ca in the classroom.</t>
+    <t>Log in with your school google account. NFB films can be played on campus without logging in. We also have an NFB Education licence and can make use of the resources available on nfb.ca in the classroom.</t>
   </si>
   <si>
     <t>National Film Board</t>
-  </si>
-  <si>
-    <t>NFB films can be played on campus without logging in (because we're using IP address authentication). We have an NFB Education licence and, therefore, can make use of the resources available on nfb.ca in the classroom.</t>
   </si>
   <si>
     <t>Nikkei Asia</t>
@@ -2593,7 +2590,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" ht="96.75" customHeight="1">
+    <row r="2" ht="63.75" customHeight="1">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
@@ -2853,7 +2850,7 @@
       <c r="A6" s="24">
         <v>3.742343E7</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="26" t="s">
         <v>114</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -3115,7 +3112,7 @@
       <c r="Y10" s="25"/>
       <c r="Z10" s="25"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="24">
         <v>3.7423435E7</v>
       </c>
@@ -3668,7 +3665,7 @@
       </c>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
-      <c r="K21" s="25" t="s">
+      <c r="K21" s="26" t="s">
         <v>198</v>
       </c>
       <c r="L21" s="25" t="s">
@@ -3685,9 +3682,7 @@
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
-      <c r="T21" s="25" t="s">
-        <v>200</v>
-      </c>
+      <c r="T21" s="25"/>
       <c r="U21" s="25"/>
       <c r="V21" s="25"/>
       <c r="W21" s="25"/>
@@ -3702,7 +3697,7 @@
         <v>3.7458513E7</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>89</v>
@@ -3711,24 +3706,24 @@
         <v>90</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F22" s="25" t="s">
         <v>92</v>
       </c>
       <c r="G22" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="H22" s="25" t="s">
         <v>203</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>204</v>
       </c>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="L22" s="25" t="s">
         <v>205</v>
-      </c>
-      <c r="L22" s="25" t="s">
-        <v>206</v>
       </c>
       <c r="M22" s="26" t="s">
         <v>96</v>
@@ -3758,7 +3753,7 @@
         <v>3.7463802E7</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>89</v>
@@ -3767,24 +3762,24 @@
         <v>90</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F23" s="25" t="s">
         <v>92</v>
       </c>
       <c r="G23" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="H23" s="25" t="s">
         <v>209</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>210</v>
       </c>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M23" s="26" t="s">
         <v>96</v>

</xml_diff>